<commit_message>
Initial Glider Design v6.0
- Python
- Flat-plate analytic aerodynamic model
- Reduce complexity of roll-in model
</commit_message>
<xml_diff>
--- a/01_Initial_Glider_Design/C_results/nausicaa_results.xlsx
+++ b/01_Initial_Glider_Design/C_results/nausicaa_results.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.384410401031462</v>
+        <v>4.143982389700622</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.00000009715565</v>
+        <v>10.00000009998912</v>
       </c>
     </row>
     <row r="4">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.79850836493705</v>
+        <v>2.500000024975229</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08921756673240951</v>
+        <v>0.1358702519941318</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7.650115599176487</v>
+        <v>5.974975678830996</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.6996465196945604</v>
+        <v>0.8466759763537778</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9.273755995297487e-09</v>
+        <v>2.627102812685198e-06</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.6996465104208044</v>
+        <v>-0.846673349250965</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.03999999043822991</v>
+        <v>0.03999998999529015</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3999999900566858</v>
+        <v>0.3999999900111381</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02950768621668346</v>
+        <v>0.04000000999922655</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>44844.12735118147</v>
+        <v>33027.94907862497</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6777602157438033</v>
+        <v>1.489473714869758</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.1012598564032433</v>
+        <v>0.1734057146235082</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.004034291352667222</v>
+        <v>0.04037606265197123</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.001350073065018612</v>
+        <v>0.05165666525041572</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.174210475205247e-15</v>
+        <v>0.8984967341029297</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-1.375810098390664e-14</v>
+        <v>3.323304392746219</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>6.593568004831516</v>
+        <v>-4.291134540853666</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.8493420848424295</v>
+        <v>1.016816387783703</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-45.26575202016993</v>
+        <v>-39.72418671720052</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.5734615754574507</v>
+        <v>0.1915576723065062</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2.196037365083999</v>
+        <v>3.946748343171597</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.4895052395440088</v>
+        <v>0.7168557603318466</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.8567552893072178</v>
+        <v>2.21277354021489</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.8493420848424295</v>
+        <v>1.016816387783703</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.0004347513903433786</v>
+        <v>0.0003026548411574736</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5.516019271195013e-11</v>
+        <v>1.506194090072323e-09</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.02140932256687558</v>
+        <v>0.02378068587467642</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-6.591058280951924e-18</v>
+        <v>-1.009948114489964e-17</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.005766434495811796</v>
+        <v>0.01992155689141272</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.001278016494057853</v>
+        <v>0.00885673998055881</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.01076649018695757</v>
+        <v>0.0009539459836602311</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.01202947022093258</v>
+        <v>0.008813731172952078</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>9.622420979361932e-21</v>
+        <v>3.332735595446488e-21</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-1.078192527405808e-05</v>
+        <v>-0.0002503571623321952</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1.294425150053429e-20</v>
+        <v>-2.280158113993334e-20</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>89.21756673240951</v>
+        <v>135.8702519941318</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.1966910658845727</v>
+        <v>0.2995426311825568</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.0310529141129299</v>
+        <v>0.04143790475840792</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.0002317130315281432</v>
+        <v>0.007336442508956208</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>6.343814529362613e-05</v>
+        <v>0.01501426640938007</v>
       </c>
     </row>
     <row r="46">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.01646080279347328</v>
+        <v>0.002149287324855123</v>
       </c>
     </row>
     <row r="51">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-9.997660589617903e-09</v>
+        <v>0.02506788788185603</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.006608708646845148</v>
+        <v>0.01006446311067643</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.04799173185776849</v>
+        <v>0.01436147517497544</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.1396647667937349</v>
+        <v>-0.2723282682330403</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-1.399934304341588e-17</v>
+        <v>9.367102447921916e-17</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>-1.401963353458585e-17</v>
+        <v>1.250826987070088e-16</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1.068451611104097</v>
+        <v>1.627154779350576</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-7.544629312224067e-18</v>
+        <v>0.06212886750254282</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.1396647667937349</v>
+        <v>0.2723282682330403</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-1.399934304341588e-17</v>
+        <v>9.367102447921916e-17</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1.033038390073349e-11</v>
+        <v>2.279535067650773e-17</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-1.341632105583915e-18</v>
+        <v>1.890877734039433e-16</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.8961678480821659</v>
+        <v>0.8921212093146058</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-6.32808649923477e-18</v>
+        <v>0.03406343459952656</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1171443537635741</v>
+        <v>0.1493095967696309</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>-1.732471439206253e-17</v>
+        <v>3.448001331619686e-17</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>5.799488968950238e-11</v>
+        <v>1.073521418550228e-16</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-1.660320271914085e-18</v>
+        <v>6.960262238131471e-17</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.05577956646567972</v>
+        <v>0.2247130993194826</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.0838852003280552</v>
+        <v>0.04761516891355775</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>4.25644495759293</v>
+        <v>2.057193054087998</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.7062590494962543</v>
+        <v>1.070697443330118</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-4.1682848788249e-13</v>
+        <v>0.002730582847392099</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-1.475180482024528e-12</v>
+        <v>0.1588345683104776</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>-0.1702577576045691</v>
+        <v>-0.08228770158190028</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>-6.457742368182611e-13</v>
+        <v>0.05388861074945468</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.02738546751285945</v>
+        <v>0.02843751652621496</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-5.258652777019424e-06</v>
+        <v>-0.002734123489764533</v>
       </c>
     </row>
     <row r="80">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>-4.356612483254874e-07</v>
+        <v>-0.01631700644930289</v>
       </c>
     </row>
     <row r="81">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.08434877355756823</v>
+        <v>-0.7042471408726034</v>
       </c>
     </row>
     <row r="82">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-0.07999999001940634</v>
+        <v>-0.07999999002034769</v>
       </c>
     </row>
     <row r="83">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-7.199049415784339e-07</v>
+        <v>0.02080043691423047</v>
       </c>
     </row>
     <row r="84">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.02999999001674997</v>
+        <v>0.02999999000122063</v>
       </c>
     </row>
     <row r="85">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-0.2196469352598872</v>
+        <v>0.087230281847203</v>
       </c>
     </row>
     <row r="86">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>-0.002882687352045998</v>
+        <v>-0.3383973704019771</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-0.001802319840968347</v>
+        <v>0.03614329957715711</v>
       </c>
     </row>
     <row r="88">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.2070844529898076</v>
+        <v>-0.1703430899706801</v>
       </c>
     </row>
     <row r="89">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-0.7037468152702296</v>
+        <v>-0.3412339681372011</v>
       </c>
     </row>
     <row r="90">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>1.49283075106188e-05</v>
+        <v>-0.06749694827949038</v>
       </c>
     </row>
     <row r="91">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-0.2708198869259493</v>
+        <v>-0.05040299875542154</v>
       </c>
     </row>
     <row r="92">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.12103926334317</v>
+        <v>0.4279711015071631</v>
       </c>
     </row>
     <row r="93">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.2761132733832827</v>
+        <v>0.2477992570826815</v>
       </c>
     </row>
     <row r="94">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>2.174325546762794e-15</v>
+        <v>-0.1542028497657569</v>
       </c>
     </row>
     <row r="95">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>5.796928197856064e-19</v>
+        <v>-0.09500434585380632</v>
       </c>
     </row>
     <row r="96">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-17.56605255996989</v>
+        <v>-1.144762810336675</v>
       </c>
     </row>
     <row r="97">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>3.234199630369877e-15</v>
+        <v>-0.02094373634167496</v>
       </c>
     </row>
     <row r="98">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-7.852797490048856e-05</v>
+        <v>-0.0698211701672946</v>
       </c>
     </row>
     <row r="99">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>-0.0003026550516455062</v>
+        <v>-0.001385994360586507</v>
       </c>
     </row>
     <row r="100">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.1544994545351264</v>
+        <v>0.05934167704105264</v>
       </c>
     </row>
     <row r="101">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.1701651444550821</v>
+        <v>0.2118940453844985</v>
       </c>
     </row>
     <row r="102">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.0005237021813549922</v>
+        <v>-0.01622367756332293</v>
       </c>
     </row>
     <row r="103">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>-0.2320288208662004</v>
+        <v>0.003837786800247243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>